<commit_message>
Renamed folder back to CustomAppBar
</commit_message>
<xml_diff>
--- a/project_features_checklist_MKKG.xlsx
+++ b/project_features_checklist_MKKG.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10212"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{778CD906-AFFF-4D45-85D5-55E0E210E750}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DE3B1AA-B7B5-A246-A03B-8ABE771C41F4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="107">
   <si>
     <t>Feature</t>
   </si>
@@ -281,9 +281,6 @@
   </si>
   <si>
     <t>Full  navigation -&gt; no buttons needed</t>
-  </si>
-  <si>
-    <t>Works almost. Only synchronous loading issues. Branch: feature/47_template_statistics_chart</t>
   </si>
   <si>
     <t>User has to be logged in.</t>
@@ -1057,8 +1054,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
-      <selection activeCell="A153" sqref="A153"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1366,28 +1363,25 @@
       </c>
       <c r="D32" s="15"/>
     </row>
-    <row r="33" spans="1:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="10"/>
       <c r="B33" s="13"/>
       <c r="C33" s="14"/>
       <c r="D33" s="14"/>
     </row>
-    <row r="34" spans="1:5" ht="53" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" ht="53" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B34" s="13">
         <v>3</v>
       </c>
-      <c r="C34" s="15"/>
-      <c r="D34" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="E34" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="36" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C34" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="D34" s="15"/>
+    </row>
+    <row r="35" spans="1:4" ht="36" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>21</v>
       </c>
@@ -1399,13 +1393,13 @@
       </c>
       <c r="D35" s="15"/>
     </row>
-    <row r="36" spans="1:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="8"/>
       <c r="B36" s="8"/>
       <c r="C36" s="14"/>
       <c r="D36" s="14"/>
     </row>
-    <row r="37" spans="1:5" ht="36" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" ht="36" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
         <v>22</v>
       </c>
@@ -1417,13 +1411,13 @@
       </c>
       <c r="D37" s="15"/>
     </row>
-    <row r="38" spans="1:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="9"/>
       <c r="B38" s="8"/>
       <c r="C38" s="14"/>
       <c r="D38" s="14"/>
     </row>
-    <row r="39" spans="1:5" ht="53" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" ht="53" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
         <v>23</v>
       </c>
@@ -1433,13 +1427,13 @@
       <c r="C39" s="15"/>
       <c r="D39" s="15"/>
     </row>
-    <row r="40" spans="1:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="10"/>
       <c r="B40" s="13"/>
       <c r="C40" s="14"/>
       <c r="D40" s="14"/>
     </row>
-    <row r="41" spans="1:5" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
         <v>24</v>
       </c>
@@ -1451,13 +1445,13 @@
       </c>
       <c r="D41" s="15"/>
     </row>
-    <row r="42" spans="1:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="8"/>
       <c r="B42" s="8"/>
       <c r="C42" s="14"/>
       <c r="D42" s="14"/>
     </row>
-    <row r="43" spans="1:5" ht="36" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" ht="36" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
         <v>25</v>
       </c>
@@ -1469,13 +1463,13 @@
       </c>
       <c r="D43" s="15"/>
     </row>
-    <row r="44" spans="1:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="9"/>
       <c r="B44" s="8"/>
       <c r="C44" s="14"/>
       <c r="D44" s="14"/>
     </row>
-    <row r="45" spans="1:5" ht="53" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" ht="53" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
         <v>26</v>
       </c>
@@ -1487,16 +1481,16 @@
       </c>
       <c r="D45" s="15"/>
     </row>
-    <row r="46" spans="1:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A46" s="10"/>
       <c r="B46" s="13"/>
       <c r="C46" s="14"/>
       <c r="D46" s="14"/>
     </row>
-    <row r="47" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="5"/>
     </row>
-    <row r="48" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="5"/>
     </row>
     <row r="49" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1541,7 +1535,7 @@
       </c>
       <c r="D53" s="15"/>
       <c r="E53" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1562,7 +1556,7 @@
       </c>
       <c r="D55" s="15"/>
       <c r="E55" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1583,7 +1577,7 @@
       </c>
       <c r="D57" s="15"/>
       <c r="E57" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1616,7 +1610,7 @@
       </c>
       <c r="D60" s="15"/>
       <c r="E60" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1877,7 +1871,7 @@
       </c>
       <c r="D92" s="15"/>
       <c r="E92" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1988,7 +1982,7 @@
       </c>
       <c r="D105" s="15"/>
       <c r="E105" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="106" spans="1:5" ht="19" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2075,7 +2069,7 @@
       </c>
       <c r="D115" s="15"/>
       <c r="E115" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="116" spans="1:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2096,7 +2090,7 @@
         <v>84</v>
       </c>
       <c r="E117" s="24" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="118" spans="1:5" ht="36" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2153,7 +2147,7 @@
       </c>
       <c r="D123" s="15"/>
       <c r="E123" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="124" spans="1:5" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2174,7 +2168,7 @@
         <v>84</v>
       </c>
       <c r="E125" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="126" spans="1:5" ht="36" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2207,7 +2201,7 @@
       </c>
       <c r="D128" s="15"/>
       <c r="E128" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="129" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -2352,7 +2346,7 @@
     </row>
     <row r="147" spans="1:5" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A147" s="27" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B147" s="19">
         <v>2</v>
@@ -2364,7 +2358,7 @@
     </row>
     <row r="148" spans="1:5" s="24" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A148" s="28" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B148" s="25">
         <v>1</v>
@@ -2376,7 +2370,7 @@
     </row>
     <row r="149" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A149" s="28" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B149" s="19">
         <v>1</v>
@@ -2388,7 +2382,7 @@
     </row>
     <row r="150" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A150" s="28" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B150" s="19">
         <v>1</v>
@@ -2400,7 +2394,7 @@
     </row>
     <row r="151" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A151" s="28" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B151" s="19">
         <v>2</v>
@@ -2412,7 +2406,7 @@
     </row>
     <row r="152" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A152" s="28" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B152" s="19">
         <v>5</v>
@@ -2424,7 +2418,7 @@
     </row>
     <row r="153" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A153" s="28" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B153" s="19">
         <v>2</v>
@@ -2436,7 +2430,7 @@
     </row>
     <row r="154" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A154" s="28" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B154" s="19">
         <v>3</v>
@@ -2448,7 +2442,7 @@
     </row>
     <row r="155" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A155" s="28" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B155" s="19">
         <v>1</v>

</xml_diff>